<commit_message>
Create Mahjong Tile Set graphics
</commit_message>
<xml_diff>
--- a/frontend/frontend-timelog.xlsx
+++ b/frontend/frontend-timelog.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="12">
   <si>
     <t xml:space="preserve">Total hours:</t>
   </si>
@@ -53,6 +53,9 @@
   </si>
   <si>
     <t xml:space="preserve">Github ongelmia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Laatta grafiikat</t>
   </si>
 </sst>
 </file>
@@ -130,7 +133,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -152,6 +155,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -278,10 +285,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
+      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -295,7 +302,7 @@
       </c>
       <c r="B1" s="1" t="n">
         <f aca="false">SUM(D:D)</f>
-        <v>0.666666666666667</v>
+        <v>0.875</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -466,10 +473,67 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="4"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="3"/>
+      <c r="A11" s="4" t="n">
+        <v>46039</v>
+      </c>
+      <c r="B11" s="1" t="n">
+        <v>0.791666666666667</v>
+      </c>
+      <c r="C11" s="1" t="n">
+        <v>0.854166666666667</v>
+      </c>
+      <c r="D11" s="5" t="n">
+        <f aca="false">C11-B11</f>
+        <v>0.0625</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="6" t="n">
+        <v>46040</v>
+      </c>
+      <c r="B12" s="1" t="n">
+        <v>0.895833333333333</v>
+      </c>
+      <c r="C12" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D12" s="5" t="n">
+        <f aca="false">C12-B12</f>
+        <v>0.104166666666667</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="6" t="n">
+        <v>46041</v>
+      </c>
+      <c r="B13" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C13" s="1" t="n">
+        <v>0.0416666666666667</v>
+      </c>
+      <c r="D13" s="5" t="n">
+        <f aca="false">C13-B13</f>
+        <v>0.0416666666666667</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>11</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>